<commit_message>
Now committing excel file
</commit_message>
<xml_diff>
--- a/Excel_file.xlsx
+++ b/Excel_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\46698\Desktop\Git_repos\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722F55FF-C4FB-470C-A8AD-F72BD6881293}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E98FE0-4DF3-4FB1-AA0F-5916B36A80D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Version 1</t>
+    <t>Version 2</t>
   </si>
 </sst>
 </file>
@@ -347,9 +347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>